<commit_message>
exception handling need to be modified
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\srika\OneDrive\Documents\UiPath\Invoice Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90DBD48D-B775-4ECF-B1DE-3097D190CB3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E01D53-CDCB-462C-B790-9B9A0FD70103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -181,6 +181,33 @@
   </si>
   <si>
     <t>Liable tax percent</t>
+  </si>
+  <si>
+    <t>Statuspaid</t>
+  </si>
+  <si>
+    <t>Paid</t>
+  </si>
+  <si>
+    <t>StatusUnPaid</t>
+  </si>
+  <si>
+    <t>Unpaid</t>
+  </si>
+  <si>
+    <t>StatusPartiallyPaid</t>
+  </si>
+  <si>
+    <t>Partially Paid</t>
+  </si>
+  <si>
+    <t>StatusOverDue</t>
+  </si>
+  <si>
+    <t>Overdue</t>
+  </si>
+  <si>
+    <t>Payment status matching with status dropdown in ERP</t>
   </si>
 </sst>
 </file>
@@ -577,7 +604,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -686,10 +713,50 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>